<commit_message>
small fix in example dataset for 1961. Small fix for imbalance computations....
</commit_message>
<xml_diff>
--- a/example/production france.xlsx
+++ b/example/production france.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D786189B-545C-43C2-8DBB-1C94F6EF2590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE510970-B8F3-4911-8AD7-541BDD59CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -806,9 +806,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
   <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -851,7 +851,7 @@
         <v>61</v>
       </c>
       <c r="E2">
-        <v>5412.79</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -868,7 +868,7 @@
         <v>62</v>
       </c>
       <c r="E3">
-        <v>2480</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -919,7 +919,7 @@
         <v>65</v>
       </c>
       <c r="E6">
-        <v>95730.52</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -936,7 +936,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="1">
-        <v>20000</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -3876,8 +3876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4044,7 +4044,7 @@
         <v>37</v>
       </c>
       <c r="B15">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="C15" t="s">
         <v>67</v>
@@ -4066,7 +4066,7 @@
         <v>37</v>
       </c>
       <c r="B17">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="C17" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
Minor upgrades in documentations (input, engine and index). Change the...
</commit_message>
<xml_diff>
--- a/example/production france.xlsx
+++ b/example/production france.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faustega\Documents\These\isterre-dynamic-modeling\grafs-e-project\grafs-e\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE510970-B8F3-4911-8AD7-541BDD59CBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94CF26D-6000-43E4-8177-037D6DAE8DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F475FEA0-B9E5-4A03-9EDE-4A3E6C5C262C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="77">
   <si>
     <t>Area</t>
   </si>
@@ -804,11 +804,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D825A9-0C1C-44E4-98B7-F194F26ABDB6}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136:XFD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3120,16 +3120,16 @@
         <v>5</v>
       </c>
       <c r="B136">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E136">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
@@ -3143,10 +3143,10 @@
         <v>36</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E137">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
@@ -3160,10 +3160,10 @@
         <v>36</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E138">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
@@ -3171,16 +3171,16 @@
         <v>5</v>
       </c>
       <c r="B139">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E139">
-        <v>0.05</v>
+        <v>71</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
@@ -3188,7 +3188,7 @@
         <v>5</v>
       </c>
       <c r="B140">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>36</v>
@@ -3197,7 +3197,7 @@
         <v>71</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
@@ -3208,13 +3208,13 @@
         <v>2023</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>73</v>
+        <v>26</v>
+      </c>
+      <c r="D141" t="s">
+        <v>14</v>
+      </c>
+      <c r="E141" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
@@ -3228,10 +3228,10 @@
         <v>26</v>
       </c>
       <c r="D142" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E142" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
@@ -3245,10 +3245,10 @@
         <v>26</v>
       </c>
       <c r="D143" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E143" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
@@ -3256,16 +3256,16 @@
         <v>5</v>
       </c>
       <c r="B144">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D144" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E144" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
@@ -3279,10 +3279,10 @@
         <v>26</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E145" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
@@ -3296,162 +3296,162 @@
         <v>26</v>
       </c>
       <c r="D146" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E146" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A147" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B147">
-        <v>1961</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D147" t="s">
-        <v>21</v>
-      </c>
-      <c r="E147" t="s">
-        <v>39</v>
+      <c r="A147" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E147" s="9">
+        <v>2.76</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A148" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B148" s="2">
-        <v>1961</v>
-      </c>
-      <c r="C148" s="5" t="s">
+      <c r="A148" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1961</v>
+      </c>
+      <c r="C148" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D148" s="5" t="s">
-        <v>69</v>
+      <c r="D148" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="E148" s="9">
-        <v>2.76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A149" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B149" s="3">
-        <v>1961</v>
-      </c>
-      <c r="C149" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D149" s="6" t="s">
-        <v>62</v>
+      <c r="A149" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B149" s="2">
+        <v>1961</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E149" s="9">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A150" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B150" s="2">
+      <c r="A150" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B150" s="3">
         <v>1961</v>
       </c>
       <c r="C150" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D150" s="5" t="s">
-        <v>6</v>
+      <c r="D150" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E150" s="9">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A151" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B151" s="3">
+      <c r="A151" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B151" s="2">
         <v>1961</v>
       </c>
       <c r="C151" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D151" s="6" t="s">
-        <v>68</v>
+      <c r="D151" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E151" s="9">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A152" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B152" s="2">
+      <c r="A152" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B152" s="3">
         <v>1961</v>
       </c>
       <c r="C152" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D152" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E152" s="9">
-        <v>2.2000000000000002</v>
+      <c r="D152" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A153" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B153" s="3">
+      <c r="A153" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B153" s="2">
         <v>1961</v>
       </c>
       <c r="C153" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D153" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E153" s="4">
-        <v>0</v>
+      <c r="D153" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" s="9">
+        <v>3.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A154" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B154" s="2">
+      <c r="A154" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="3">
         <v>1961</v>
       </c>
       <c r="C154" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D154" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E154" s="9">
-        <v>3.5</v>
+      <c r="D154" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E154" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A155" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B155" s="3">
+      <c r="A155" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" s="2">
         <v>1961</v>
       </c>
       <c r="C155" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D155" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E155" s="12">
+      <c r="D155" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E155" s="13">
         <v>0</v>
       </c>
     </row>
@@ -3460,117 +3460,117 @@
         <v>5</v>
       </c>
       <c r="B156" s="2">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E156" s="13">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="E156" s="9">
+        <v>2.5</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A157" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B157" s="2">
+      <c r="A157" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B157" s="3">
         <v>2023</v>
       </c>
       <c r="C157" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D157" s="5" t="s">
-        <v>6</v>
+      <c r="D157" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E157" s="9">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A158" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B158" s="3">
+      <c r="A158" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" s="2">
         <v>2023</v>
       </c>
       <c r="C158" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D158" s="6" t="s">
-        <v>68</v>
+      <c r="D158" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E158" s="9">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A159" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B159" s="2">
+      <c r="A159" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" s="3">
         <v>2023</v>
       </c>
       <c r="C159" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D159" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E159" s="9">
-        <v>2.2000000000000002</v>
+      <c r="D159" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A160" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B160" s="3">
+      <c r="A160" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B160" s="2">
         <v>2023</v>
       </c>
       <c r="C160" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D160" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E160" s="4">
-        <v>0</v>
+      <c r="D160" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160" s="9">
+        <v>3.5</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A161" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B161" s="2">
+      <c r="A161" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161" s="3">
         <v>2023</v>
       </c>
       <c r="C161" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D161" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E161" s="9">
-        <v>3.5</v>
+      <c r="D161" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E161" s="12">
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A162" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B162" s="3">
+      <c r="A162" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="2">
         <v>2023</v>
       </c>
       <c r="C162" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D162" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E162" s="12">
+      <c r="D162" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="13">
         <v>0</v>
       </c>
     </row>
@@ -3579,118 +3579,118 @@
         <v>5</v>
       </c>
       <c r="B163" s="2">
-        <v>2023</v>
+        <v>1961</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E163" s="13">
+        <v>6</v>
+      </c>
+      <c r="E163">
         <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B164" s="2">
+      <c r="A164" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="3">
         <v>1961</v>
       </c>
       <c r="C164" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D164" s="5" t="s">
-        <v>6</v>
+      <c r="D164" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E164">
         <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A165" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B165" s="3">
+      <c r="A165" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" s="2">
         <v>1961</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D165" s="6" t="s">
-        <v>68</v>
+      <c r="D165" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E165">
         <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A166" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B166" s="2">
+      <c r="A166" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="3">
         <v>1961</v>
       </c>
       <c r="C166" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D166" s="5" t="s">
-        <v>7</v>
+      <c r="D166" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A167" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B167" s="3">
+      <c r="A167" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" s="2">
         <v>1961</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D167" s="6" t="s">
-        <v>8</v>
+      <c r="D167" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E167">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A168" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B168" s="2">
+      <c r="A168" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="3">
         <v>1961</v>
       </c>
       <c r="C168" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D168" s="5" t="s">
-        <v>9</v>
+      <c r="D168" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E168">
         <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A169" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B169" s="3">
+      <c r="A169" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="2">
         <v>1961</v>
       </c>
       <c r="C169" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D169" s="6" t="s">
-        <v>11</v>
+      <c r="D169" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
@@ -3698,135 +3698,135 @@
         <v>5</v>
       </c>
       <c r="B170" s="2">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E170">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A171" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B171" s="2">
+      <c r="A171" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" s="3">
         <v>2023</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D171" s="5" t="s">
-        <v>6</v>
+      <c r="D171" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A172" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B172" s="3">
+      <c r="A172" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="2">
         <v>2023</v>
       </c>
       <c r="C172" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D172" s="6" t="s">
-        <v>68</v>
+      <c r="D172" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E172">
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A173" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B173" s="2">
+      <c r="A173" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="3">
         <v>2023</v>
       </c>
       <c r="C173" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D173" s="5" t="s">
-        <v>7</v>
+      <c r="D173" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A174" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B174" s="3">
+      <c r="A174" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="2">
         <v>2023</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D174" s="6" t="s">
-        <v>8</v>
+      <c r="D174" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E174">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A175" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B175" s="2">
+      <c r="A175" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="3">
         <v>2023</v>
       </c>
       <c r="C175" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D175" s="5" t="s">
-        <v>9</v>
+      <c r="D175" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E175">
         <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A176" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B176" s="3">
+      <c r="A176" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="2">
         <v>2023</v>
       </c>
       <c r="C176" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D176" s="6" t="s">
-        <v>11</v>
+      <c r="D176" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E176">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A177" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B177" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C177" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D177" s="5" t="s">
-        <v>22</v>
+      <c r="A177" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="15">
+        <v>1961</v>
+      </c>
+      <c r="C177" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D177" t="s">
+        <v>40</v>
       </c>
       <c r="E177">
-        <v>150</v>
+        <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
@@ -3834,7 +3834,7 @@
         <v>5</v>
       </c>
       <c r="B178" s="15">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="C178" s="16" t="s">
         <v>12</v>
@@ -3843,23 +3843,6 @@
         <v>40</v>
       </c>
       <c r="E178">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A179" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B179" s="15">
-        <v>2023</v>
-      </c>
-      <c r="C179" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D179" t="s">
-        <v>40</v>
-      </c>
-      <c r="E179">
         <v>25</v>
       </c>
     </row>
@@ -3876,7 +3859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80ABBC0-87F2-4F7A-9036-33771C52D9AC}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>